<commit_message>
Code update on Sep 30
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indra\OneDrive\Desktop\Batch_16_Aug\Project\IA.0165.InvoiceProcessing_Performer\IA.0165.InvoiceProcessing_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\Project 1\IA.0165.InvoiceProcessing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>IA.0165.ErrorFolder</t>
   </si>
   <si>
-    <t>C:\Users\indra\OneDrive\Documents\IA.0165.InvoiceProcessing\Inputs</t>
-  </si>
-  <si>
     <t>C:\Users\indra\OneDrive\Documents\IA.0165.InvoiceProcessing\Reports</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>30000</t>
+  </si>
+  <si>
+    <t>C:\Users\Admin\Documents\UiPath\Project 1\IA.0165.InvoiceProcessing\Input\Data_proj_invoices list</t>
   </si>
 </sst>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1642,7 +1642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1770,32 +1770,32 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="6">
         <v>15000</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="6">
         <v>45000</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="6">
         <v>120000</v>
@@ -2796,8 +2796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2872,7 +2872,7 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
@@ -2883,7 +2883,7 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>